<commit_message>
v7.15 mejora disposicion de botones
v7.15 mejora disposicion de botones
</commit_message>
<xml_diff>
--- a/tests/CONTROL DE PRUEBAS v7.11.xlsx
+++ b/tests/CONTROL DE PRUEBAS v7.11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8b5d298ea5119ec0/Documentos/GitHub/GMAO-FACTORY/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_34ADD7067FBCD35338DCEABC54032EEDF587F240" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15D0EFF5-002D-4A6F-A870-C9DC45C61B43}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_34ADD7067FBCD35338DCEABC54032EEDF587F240" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C68C11D5-6735-415E-A8B5-9E6CE460047F}"/>
   <bookViews>
-    <workbookView xWindow="38250" yWindow="3780" windowWidth="24300" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-150" yWindow="-150" windowWidth="38700" windowHeight="21300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla de comprobacion de Accion" sheetId="1" r:id="rId1"/>
@@ -720,9 +720,6 @@
     <t>6. AYUDA</t>
   </si>
   <si>
-    <t>fallo</t>
-  </si>
-  <si>
     <t>⬜ ✓ BUSCA POR EL CONTENIDO DE LAS FILAS DA IGUAL QUE COLUMNA SEA</t>
   </si>
   <si>
@@ -748,13 +745,16 @@
   </si>
   <si>
     <t>comprobación de textos</t>
+  </si>
+  <si>
+    <t>⬜ ✓ Ok, .-&gt; corregido en la v7,12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -813,13 +813,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
@@ -842,7 +835,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -862,11 +855,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -881,12 +869,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -896,24 +883,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
-    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1132,19 +1113,19 @@
   </sheetPr>
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="46.42578125" customWidth="1"/>
     <col min="5" max="5" width="79.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="12.75">
       <c r="A1" s="14" t="s">
         <v>212</v>
       </c>
@@ -1161,7 +1142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="14.25">
       <c r="A2" s="15" t="s">
         <v>211</v>
       </c>
@@ -1174,7 +1155,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="14.25">
       <c r="A3" s="15" t="s">
         <v>211</v>
       </c>
@@ -1191,12 +1172,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:5" ht="12.75">
+      <c r="A4" s="9" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="15" t="s">
         <v>211</v>
       </c>
@@ -1204,7 +1185,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="14.25">
       <c r="A6" s="15" t="s">
         <v>211</v>
       </c>
@@ -1212,18 +1193,18 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="17"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="17"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="17" t="s">
+    <row r="7" spans="1:5" ht="12.75">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="12.75">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="12.75">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="14.25">
       <c r="A10" s="15" t="s">
         <v>211</v>
       </c>
@@ -1240,7 +1221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="14.25">
       <c r="A11" s="15" t="s">
         <v>211</v>
       </c>
@@ -1257,7 +1238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="14.25">
       <c r="A12" s="15" t="s">
         <v>211</v>
       </c>
@@ -1276,7 +1257,7 @@
     </row>
     <row r="13" spans="1:5" ht="39.75" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -1291,7 +1272,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="14.25">
       <c r="A14" s="15" t="s">
         <v>211</v>
       </c>
@@ -1308,7 +1289,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="14.25">
       <c r="A15" s="15" t="s">
         <v>211</v>
       </c>
@@ -1325,7 +1306,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="14.25">
       <c r="A16" s="15" t="s">
         <v>224</v>
       </c>
@@ -1342,8 +1323,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:5" ht="12.75">
+      <c r="A17" s="11" t="s">
         <v>222</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1359,8 +1340,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:5" ht="12.75">
+      <c r="A18" s="11" t="s">
         <v>222</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1376,8 +1357,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:5" ht="12.75">
+      <c r="A19" s="11" t="s">
         <v>222</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1393,8 +1374,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:5" ht="12.75">
+      <c r="A20" s="11" t="s">
         <v>222</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1410,12 +1391,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:5" ht="12.75">
+      <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="14.25">
       <c r="A22" s="15" t="s">
         <v>211</v>
       </c>
@@ -1432,7 +1413,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="14.25">
       <c r="A23" s="15" t="s">
         <v>226</v>
       </c>
@@ -1449,7 +1430,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="14.25">
       <c r="A24" s="15" t="s">
         <v>211</v>
       </c>
@@ -1466,7 +1447,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="14.25">
       <c r="A25" s="15" t="s">
         <v>227</v>
       </c>
@@ -1483,7 +1464,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="14.25">
       <c r="A26" s="15" t="s">
         <v>225</v>
       </c>
@@ -1497,8 +1478,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:5" ht="12.75">
+      <c r="A27" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1509,8 +1490,8 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="18" t="s">
+    <row r="28" spans="1:5" ht="12.75">
+      <c r="A28" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1521,8 +1502,8 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:5" ht="12.75">
+      <c r="A29" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1533,8 +1514,8 @@
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="18" t="s">
+    <row r="30" spans="1:5" ht="12.75">
+      <c r="A30" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1545,13 +1526,13 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="17" t="s">
+    <row r="31" spans="1:5" ht="12.75">
+      <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" ht="14.25">
       <c r="A32" s="15" t="s">
         <v>228</v>
       </c>
@@ -1568,7 +1549,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="14.25">
       <c r="A33" s="15" t="s">
         <v>226</v>
       </c>
@@ -1602,7 +1583,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" ht="14.25">
       <c r="A35" s="15" t="s">
         <v>229</v>
       </c>
@@ -1616,8 +1597,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="18" t="s">
+    <row r="36" spans="1:5" ht="12.75">
+      <c r="A36" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1628,8 +1609,8 @@
       </c>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:5" ht="12.75">
+      <c r="A37" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1640,8 +1621,8 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="18" t="s">
+    <row r="38" spans="1:5" ht="12.75">
+      <c r="A38" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1651,8 +1632,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="18" t="s">
+    <row r="39" spans="1:5" ht="12.75">
+      <c r="A39" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1662,8 +1643,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="17" t="s">
+    <row r="40" spans="1:5" ht="12.75">
+      <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1729,7 +1710,7 @@
         <v>72</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>73</v>
@@ -1752,9 +1733,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="17" t="s">
-        <v>233</v>
+    <row r="46" spans="1:5" ht="12.75">
+      <c r="A46" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1766,10 +1747,10 @@
         <v>229</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1779,28 +1760,28 @@
         <v>229</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="17"/>
+    <row r="49" spans="1:5" ht="12.75">
+      <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="17" t="s">
+    <row r="50" spans="1:5" ht="12.75">
+      <c r="A50" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="17" t="s">
+    <row r="51" spans="1:5" ht="12.75">
+      <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1816,8 +1797,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="17" t="s">
+    <row r="52" spans="1:5" ht="12.75">
+      <c r="A52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1833,8 +1814,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="17" t="s">
+    <row r="53" spans="1:5" ht="12.75">
+      <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1850,8 +1831,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="17" t="s">
+    <row r="54" spans="1:5" ht="12.75">
+      <c r="A54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -1864,9 +1845,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="19" t="s">
-        <v>231</v>
+    <row r="55" spans="1:5" ht="14.25">
+      <c r="A55" s="15" t="s">
+        <v>240</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>77</v>
@@ -1878,7 +1859,7 @@
       <c r="E55" s="10"/>
     </row>
     <row r="56" spans="1:5" ht="12.75">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1891,7 +1872,7 @@
       <c r="E56" s="10"/>
     </row>
     <row r="57" spans="1:5" ht="12.75">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -1904,7 +1885,7 @@
       <c r="E57" s="10"/>
     </row>
     <row r="58" spans="1:5" ht="12.75">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -1917,7 +1898,7 @@
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" ht="12.75">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -1929,13 +1910,13 @@
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="17" t="s">
+    <row r="60" spans="1:5" ht="12.75">
+      <c r="A60" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="17" t="s">
+    <row r="61" spans="1:5" ht="12.75">
+      <c r="A61" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -1951,8 +1932,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="17" t="s">
+    <row r="62" spans="1:5" ht="12.75">
+      <c r="A62" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1968,8 +1949,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="17" t="s">
+    <row r="63" spans="1:5" ht="12.75">
+      <c r="A63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -1985,8 +1966,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="17" t="s">
+    <row r="64" spans="1:5" ht="12.75">
+      <c r="A64" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2003,47 +1984,47 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A66" s="17"/>
+      <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A69" s="17"/>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="17" t="s">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" ht="12.75">
+      <c r="A70" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="17" t="s">
+    <row r="71" spans="1:5" ht="12.75">
+      <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B71" s="1" t="s">

</xml_diff>